<commit_message>
utility updated and appreciate flow changes
</commit_message>
<xml_diff>
--- a/RR/excel/NominationFlow/NominationFlow.xlsx
+++ b/RR/excel/NominationFlow/NominationFlow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="7"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="C943" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,8 @@
     <sheet name="C924" sheetId="6" r:id="rId6"/>
     <sheet name="C1270" sheetId="7" r:id="rId7"/>
     <sheet name="C1328" sheetId="9" r:id="rId8"/>
-    <sheet name="C999" sheetId="8" r:id="rId9"/>
+    <sheet name="C1291" sheetId="10" r:id="rId9"/>
+    <sheet name="C999" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="68">
   <si>
     <t>Tata Steel</t>
   </si>
@@ -194,6 +195,33 @@
   </si>
   <si>
     <t>Advantage!1328</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>american-airlines.nominator@yopmail.com</t>
+  </si>
+  <si>
+    <t>american-airlines.requestor@yopmail.com</t>
+  </si>
+  <si>
+    <t>american-airlines.approver@yopmail.com</t>
+  </si>
+  <si>
+    <t>american-airlines.exception@yopmail.com</t>
+  </si>
+  <si>
+    <t>superuser.igtph@yopmail.com</t>
+  </si>
+  <si>
+    <t>american-airlines.user1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Advantage!1291</t>
   </si>
   <si>
     <t>Celio</t>
@@ -1294,6 +1322,89 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.1388888888889" customWidth="1"/>
+    <col min="2" max="2" width="17.4259259259259" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="5" width="21.712962962963" customWidth="1"/>
+    <col min="6" max="6" width="19.5740740740741" customWidth="1"/>
+    <col min="7" max="7" width="17.5740740740741" customWidth="1"/>
+    <col min="8" max="8" width="20.8518518518519" customWidth="1"/>
+    <col min="9" max="9" width="22.287037037037" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="9:9">
+      <c r="I1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" ht="28.8" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -1954,8 +2065,8 @@
   <sheetPr/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2077,14 +2188,14 @@
   <sheetPr/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.1388888888889" customWidth="1"/>
-    <col min="2" max="2" width="17.4259259259259" customWidth="1"/>
+    <col min="2" max="2" width="23.2222222222222" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="5" width="21.712962962963" customWidth="1"/>
     <col min="6" max="6" width="19.5740740740741" customWidth="1"/>
@@ -2095,7 +2206,7 @@
   <sheetData>
     <row r="1" spans="9:9">
       <c r="I1" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2103,10 +2214,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -2115,10 +2226,25 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" ht="28.8" spans="1:4">
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" ht="43.2" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2131,25 +2257,51 @@
       <c r="D7" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" display="superuser.igtph@yopmail.com" tooltip="mailto:superuser.igtph@yopmail.com"/>
+    <hyperlink ref="G7" r:id="rId2" display="american-airlines.user1@yopmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>